<commit_message>
## 2025-05-12 ### Ajouts - Ajout des champs `chsta_codehydro`, `chsta_codemeteofrance`, `chsta_infl_ant_type`, `chsta_infl_nappe` dans le fichier excel des stations
</commit_message>
<xml_diff>
--- a/data/Stations/Saisie_stations_chroniques_avec_champs_complementaires.xlsx
+++ b/data/Stations/Saisie_stations_chroniques_avec_champs_complementaires.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Fixe-FD39/Nextcloud_FD/NAS-JB/Outils/Physico-chimie/Thermie/Fiches_notices/Notice/notice-thermie/data/Stations/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jean-baptistefagot/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45D851E-D001-B34C-84DF-4FB6D2CA3960}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2364BC-E447-6440-88D6-CD4139028D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="19760" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="39900" windowHeight="17660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formulaire" sheetId="1" r:id="rId1"/>
@@ -122,17 +122,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>chsta_coderhj</t>
   </si>
   <si>
-    <t>Version3</t>
-  </si>
-  <si>
-    <t>2018-10-30</t>
-  </si>
-  <si>
     <t>chsta_codemo</t>
   </si>
   <si>
@@ -248,6 +242,24 @@
   </si>
   <si>
     <t>chsta_sprep</t>
+  </si>
+  <si>
+    <t>chsta_infl_ant_type</t>
+  </si>
+  <si>
+    <t>chsta_infl_nappe</t>
+  </si>
+  <si>
+    <t>chsta_codehydro</t>
+  </si>
+  <si>
+    <t>chsta_codemeteofrance</t>
+  </si>
+  <si>
+    <t>2025-05-12</t>
+  </si>
+  <si>
+    <t>Version4</t>
   </si>
 </sst>
 </file>
@@ -316,10 +328,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -677,11 +690,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T5" sqref="T5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AR1" sqref="AR1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -722,126 +735,138 @@
     <col min="36" max="36" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
+        <v>39</v>
+      </c>
+      <c r="U1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="V1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" t="s">
+      <c r="W1" t="s">
+        <v>17</v>
+      </c>
+      <c r="X1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" t="s">
         <v>37</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="AH1" t="s">
         <v>38</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AI1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AR1" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="U1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" t="s">
-        <v>18</v>
-      </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -855,17 +880,17 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
## 2025-05-14 ### Ajouts - Ajout d'explications manquantes de champs dans le fichier excel des stations - Actualisation des structures de données suite à MAJ dans `aquatools` (`0.0.174`)   * Ajout du champs `chmes_referentiel_temporel` dans les champs associés aux mesures   * Ajout des champs `chsta_codehydro`, `chsta_codemeteofrance`, `chsta_infl_ant_type`, `chsta_infl_nappe` dans les champs associés aux stations
### Modifications
- Modification de la position des champs `chsta_codehydro`, `chsta_codemeteofrance`, `chsta_infl_ant_type`, `chsta_infl_nappe` dans le fichier excel des stations
- Renommage dans jeux de données `chronique_exemple`, `chronique_structure` et `chronique_structure_hors_bdd` de `suivi_structure` par `suivis_structure` pour harmonisation

### Corrections
- Corrections de la description du champs `chsta_infl_nappe` dans les champs des stations
</commit_message>
<xml_diff>
--- a/data/Stations/Saisie_stations_chroniques_avec_champs_complementaires.xlsx
+++ b/data/Stations/Saisie_stations_chroniques_avec_champs_complementaires.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jean-baptistefagot/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jean-baptistefagot/Nextcloud/NAS-JB/Outils/Physico-chimie/Thermie/Fiches_notices/Notice/notice-thermie/data/Stations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2364BC-E447-6440-88D6-CD4139028D6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D3C1A94-1154-694C-BDDA-2ACFC3A0CDAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="39900" windowHeight="17660" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,8 +17,8 @@
     <sheet name="Àpropos" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Modèle_saisie_stations" localSheetId="0">Formulaire!$A$1:$AE$1</definedName>
-    <definedName name="Modèle_saisie_stations_1" localSheetId="0">Formulaire!$A$1:$AK$1</definedName>
+    <definedName name="Modèle_saisie_stations" localSheetId="0">Formulaire!$A$1:$AI$1</definedName>
+    <definedName name="Modèle_saisie_stations_1" localSheetId="0">Formulaire!$A$1:$AO$1</definedName>
   </definedNames>
   <calcPr calcId="140000"/>
   <extLst>
@@ -328,11 +328,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -361,11 +360,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Modèle_saisie_stations_1" connectionId="2" xr16:uid="{8E8ED82D-18DB-F042-A183-44652B0F3B69}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Modèle_saisie_stations" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Modèle_saisie_stations" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Modèle_saisie_stations_1" connectionId="2" xr16:uid="{8E8ED82D-18DB-F042-A183-44652B0F3B69}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -694,7 +693,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AR1" sqref="AR1"/>
+      <selection pane="topRight" activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -713,26 +712,28 @@
     <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.6640625" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="34" width="10.5" customWidth="1"/>
-    <col min="35" max="35" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.83203125" customWidth="1"/>
+    <col min="18" max="18" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6640625" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="14.33203125" customWidth="1"/>
+    <col min="34" max="34" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="10.5" customWidth="1"/>
+    <col min="39" max="39" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.2">
@@ -782,91 +783,91 @@
         <v>14</v>
       </c>
       <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R1" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>34</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>35</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>39</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH1" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AI1" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AJ1" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AK1" t="s">
         <v>37</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AL1" t="s">
         <v>38</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AM1" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AN1" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AO1" t="s">
         <v>29</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AP1" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AQ1" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AR1" t="s">
         <v>32</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AQ1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AR1" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>